<commit_message>
Finalized analyses. May need to make more plots (?)
</commit_message>
<xml_diff>
--- a/Lab5_MultLogRgrsn-ModSlxn/covariates-and-models.xlsx
+++ b/Lab5_MultLogRgrsn-ModSlxn/covariates-and-models.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11820" windowHeight="4410" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11820" windowHeight="4410" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="covs" sheetId="1" r:id="rId1"/>
-    <sheet name="models" sheetId="2" r:id="rId2"/>
+    <sheet name="mods" sheetId="2" r:id="rId2"/>
+    <sheet name="covmod-comp" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="80">
   <si>
     <t>elk</t>
   </si>
@@ -232,6 +233,39 @@
   </si>
   <si>
     <t>prefprey*closed + human*closed</t>
+  </si>
+  <si>
+    <t>prey</t>
+  </si>
+  <si>
+    <t>closed</t>
+  </si>
+  <si>
+    <t>prey*closed</t>
+  </si>
+  <si>
+    <t>MCPall</t>
+  </si>
+  <si>
+    <t>KDEalla</t>
+  </si>
+  <si>
+    <t>KDEallb</t>
+  </si>
+  <si>
+    <t>BVb</t>
+  </si>
+  <si>
+    <t>RDb</t>
+  </si>
+  <si>
+    <t>RDc</t>
+  </si>
+  <si>
+    <t>BVa</t>
+  </si>
+  <si>
+    <t>RDa</t>
   </si>
 </sst>
 </file>
@@ -989,8 +1023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1125,4 +1159,193 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="C2">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="D2">
+        <v>1.3</v>
+      </c>
+      <c r="E2">
+        <v>1.28</v>
+      </c>
+      <c r="F2">
+        <v>0.78</v>
+      </c>
+      <c r="G2">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>-2E-3</v>
+      </c>
+      <c r="C3">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+      <c r="D3">
+        <v>-2E-3</v>
+      </c>
+      <c r="E3">
+        <v>-4.0000000000000001E-3</v>
+      </c>
+      <c r="F3">
+        <v>-1E-3</v>
+      </c>
+      <c r="G3">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+      <c r="H3">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+      <c r="I3">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4">
+        <v>-0.75</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4">
+        <v>-1.01</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4">
+        <v>-0.1</v>
+      </c>
+      <c r="H4">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="I4">
+        <v>-0.72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6">
+        <v>2E-3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6">
+        <v>2E-3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6">
+        <v>2E-3</v>
+      </c>
+      <c r="H6">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="I6">
+        <v>2E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>